<commit_message>
Analysis on avoided costs benefit
</commit_message>
<xml_diff>
--- a/Opal Lakes Dropbear Conservation Park.xlsx
+++ b/Opal Lakes Dropbear Conservation Park.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004548DF-442C-1347-8FC5-C8058F068784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64070C0D-C530-A844-B6DE-E70349163A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1935,14 +1935,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>97776</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>125090</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>27312</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>507794</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>81936</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>27313</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1957,8 +1957,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11514120" y="8018208"/>
-          <a:ext cx="6678083" cy="666954"/>
+          <a:off x="11514120" y="7920430"/>
+          <a:ext cx="6678083" cy="1092474"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2016,6 +2016,31 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Annual cost of dropbear impact of $20 million incurred by NSW farmers. Not relevant for analysis as this cost has been superseded by the Volunteer Brigade.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:pPr algn="just"/>
           <a:endParaRPr lang="en-AU" sz="1100" b="0"/>
         </a:p>
@@ -2028,13 +2053,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>122903</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>27312</xdr:rowOff>
+      <xdr:rowOff>122903</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>532921</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>122904</xdr:rowOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>27312</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2049,7 +2074,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11539247" y="8821721"/>
+          <a:off x="11539247" y="9108494"/>
           <a:ext cx="6678083" cy="2007420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3735,8 +3760,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Asset residula value analysis
</commit_message>
<xml_diff>
--- a/Opal Lakes Dropbear Conservation Park.xlsx
+++ b/Opal Lakes Dropbear Conservation Park.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64070C0D-C530-A844-B6DE-E70349163A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFBB951-5605-3C40-A333-DBB652BFF851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="DiscountRate">[1]Parameters!$C$8</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="103">
   <si>
     <t>Source</t>
   </si>
@@ -330,18 +331,6 @@
     <t>Avoided cost operating Brigade</t>
   </si>
   <si>
-    <t>Fencing</t>
-  </si>
-  <si>
-    <t>Holding pens</t>
-  </si>
-  <si>
-    <t>Viewing platforms</t>
-  </si>
-  <si>
-    <t>Year 0 ($'000) 21/22</t>
-  </si>
-  <si>
     <t>Total Benefit</t>
   </si>
   <si>
@@ -355,13 +344,19 @@
   </si>
   <si>
     <t>Labour</t>
+  </si>
+  <si>
+    <t>Asset life (years)</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -372,6 +367,7 @@
     <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00_-;\(&quot;$&quot;#,##0.00\);\-_;"/>
     <numFmt numFmtId="171" formatCode="#,##0_-;\(#,##0\);\-_;"/>
+    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0_-;\(&quot;$&quot;#,##0\);\-_;"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -854,7 +850,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -972,7 +968,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="15" fillId="0" borderId="9" xfId="9" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="16" fillId="0" borderId="9" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="9" xfId="9" applyNumberFormat="1" applyFont="1"/>
@@ -989,6 +984,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Bad 2" xfId="1" xr:uid="{B03EBECC-4434-4525-8FB0-19D98432DF3E}"/>
@@ -2050,350 +2054,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>122903</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>122903</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>532921</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>27312</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68E565B5-157B-E044-93B6-41E04E2FE4E6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11539247" y="9108494"/>
-          <a:ext cx="6678083" cy="2007420"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Assets, including fencing, holding pens, and viewing platforms, are expected to last for </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>5 years</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> due to heavy damage caused by dropbears.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Additional capital expenditures (capex) for these assets in Year 1 (2022/23) are as follows:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="1"/>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Fencing</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: $2 million</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="1"/>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Holding pens</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: $2 million</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="1"/>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Viewing platforms</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: $3 million</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>These assets will also be depreciated over </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>5 years</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>, starting from Year 1.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>At the end of the 5-year analysis period, the estimated scrap values are:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="1"/>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Fencing</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: $400 thousand</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="1"/>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Holding pens</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: $400 thousand</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="1"/>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Viewing platforms</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: $600 thousand</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="just"/>
-          <a:endParaRPr lang="en-AU" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1379247</xdr:colOff>
       <xdr:row>56</xdr:row>
@@ -2562,6 +2222,36 @@
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
       <sheetData sheetId="28"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Notes"/>
+      <sheetName val="Economic Data and Calculations"/>
+      <sheetName val="CapEx and Funding"/>
+      <sheetName val="Cost-Benefit Analysis"/>
+      <sheetName val="Minister Brief (sample answers)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="14">
+          <cell r="F14">
+            <v>160.84</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3760,8 +3450,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4037,7 +3727,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B26" s="56" t="s">
         <v>88</v>
@@ -4065,23 +3755,23 @@
       <c r="B27" s="11">
         <v>200</v>
       </c>
-      <c r="C27" s="65">
+      <c r="C27" s="64">
         <f>$B27*2*C22</f>
         <v>40000</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="64">
         <f t="shared" ref="D27:G27" si="1">$B27*2*D22</f>
         <v>80000</v>
       </c>
-      <c r="E27" s="65">
+      <c r="E27" s="64">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="F27" s="65">
+      <c r="F27" s="64">
         <f t="shared" si="1"/>
         <v>112000</v>
       </c>
-      <c r="G27" s="65">
+      <c r="G27" s="64">
         <f t="shared" si="1"/>
         <v>120000</v>
       </c>
@@ -4093,23 +3783,23 @@
       <c r="B28" s="11">
         <v>100</v>
       </c>
-      <c r="C28" s="65">
+      <c r="C28" s="64">
         <f t="shared" ref="C28:G29" si="2">$B28*2*C23</f>
         <v>10000</v>
       </c>
-      <c r="D28" s="65">
+      <c r="D28" s="64">
         <f t="shared" si="2"/>
         <v>20000</v>
       </c>
-      <c r="E28" s="65">
+      <c r="E28" s="64">
         <f t="shared" si="2"/>
         <v>25000</v>
       </c>
-      <c r="F28" s="65">
+      <c r="F28" s="64">
         <f t="shared" si="2"/>
         <v>28000</v>
       </c>
-      <c r="G28" s="65">
+      <c r="G28" s="64">
         <f t="shared" si="2"/>
         <v>30000</v>
       </c>
@@ -4121,23 +3811,23 @@
       <c r="B29" s="11">
         <v>300</v>
       </c>
-      <c r="C29" s="65">
+      <c r="C29" s="64">
         <f t="shared" si="2"/>
         <v>90000</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="64">
         <f t="shared" si="2"/>
         <v>180000</v>
       </c>
-      <c r="E29" s="65">
+      <c r="E29" s="64">
         <f t="shared" si="2"/>
         <v>225000</v>
       </c>
-      <c r="F29" s="65">
+      <c r="F29" s="64">
         <f t="shared" si="2"/>
         <v>252000</v>
       </c>
-      <c r="G29" s="65">
+      <c r="G29" s="64">
         <f t="shared" si="2"/>
         <v>270000</v>
       </c>
@@ -4145,32 +3835,32 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="66">
+        <v>96</v>
+      </c>
+      <c r="C30" s="65">
         <f>SUM(C27:C29)</f>
         <v>140000</v>
       </c>
-      <c r="D30" s="66">
+      <c r="D30" s="65">
         <f t="shared" ref="D30:G30" si="3">SUM(D27:D29)</f>
         <v>280000</v>
       </c>
-      <c r="E30" s="66">
+      <c r="E30" s="65">
         <f t="shared" si="3"/>
         <v>350000</v>
       </c>
-      <c r="F30" s="66">
+      <c r="F30" s="65">
         <f t="shared" si="3"/>
         <v>392000</v>
       </c>
-      <c r="G30" s="66">
+      <c r="G30" s="65">
         <f t="shared" si="3"/>
         <v>420000</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="57" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B32" s="58" t="s">
         <v>89</v>
@@ -4187,93 +3877,93 @@
       <c r="F32" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="G32" s="68"/>
+      <c r="G32" s="67"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" s="65">
+        <v>99</v>
+      </c>
+      <c r="B33" s="64">
         <f>(C27+C28)*0.09</f>
         <v>4500</v>
       </c>
-      <c r="C33" s="65">
+      <c r="C33" s="64">
         <f t="shared" ref="C33:F33" si="4">(D27+D28)*0.09</f>
         <v>9000</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="64">
         <f t="shared" si="4"/>
         <v>11250</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="64">
         <f t="shared" si="4"/>
         <v>12600</v>
       </c>
-      <c r="F33" s="65">
+      <c r="F33" s="64">
         <f t="shared" si="4"/>
         <v>13500</v>
       </c>
-      <c r="G33" s="70"/>
+      <c r="G33" s="69"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" s="67">
+        <v>100</v>
+      </c>
+      <c r="B34" s="66">
         <f>(C27+C28)*0.11</f>
         <v>5500</v>
       </c>
-      <c r="C34" s="67">
+      <c r="C34" s="66">
         <f t="shared" ref="C34:F34" si="5">(D27+D28)*0.11</f>
         <v>11000</v>
       </c>
-      <c r="D34" s="67">
+      <c r="D34" s="66">
         <f t="shared" si="5"/>
         <v>13750</v>
       </c>
-      <c r="E34" s="67">
+      <c r="E34" s="66">
         <f t="shared" si="5"/>
         <v>15400</v>
       </c>
-      <c r="F34" s="67">
+      <c r="F34" s="66">
         <f t="shared" si="5"/>
         <v>16500</v>
       </c>
-      <c r="G34" s="70"/>
+      <c r="G34" s="69"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="66">
+        <v>96</v>
+      </c>
+      <c r="B35" s="65">
         <f>SUM(B33:B34)</f>
         <v>10000</v>
       </c>
-      <c r="C35" s="66">
+      <c r="C35" s="65">
         <f>SUM(C33:C34)</f>
         <v>20000</v>
       </c>
-      <c r="D35" s="66">
+      <c r="D35" s="65">
         <f>SUM(D33:D34)</f>
         <v>25000</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <f>SUM(E33:E34)</f>
         <v>28000</v>
       </c>
-      <c r="F35" s="66">
+      <c r="F35" s="65">
         <f>SUM(F33:F34)</f>
         <v>30000</v>
       </c>
-      <c r="G35" s="70"/>
+      <c r="G35" s="69"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="68"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
@@ -4340,156 +4030,89 @@
       <c r="G47" s="36"/>
       <c r="H47" s="36"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="C48" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="E48" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="F48" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48" s="58" t="s">
-        <v>93</v>
-      </c>
+    <row r="48" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B49" s="35">
-        <f>38000000/1000</f>
-        <v>38000</v>
-      </c>
-      <c r="C49" s="35">
-        <f>$B$49/5*(5-C$52)+2000/5*(5-C$52+1)</f>
-        <v>32400</v>
-      </c>
-      <c r="D49" s="35">
-        <f t="shared" ref="D49:G49" si="7">$B$49/5*(5-D$52)+2000/5*(5-D$52+1)</f>
-        <v>24400</v>
-      </c>
-      <c r="E49" s="35">
-        <f t="shared" si="7"/>
-        <v>16400</v>
-      </c>
-      <c r="F49" s="35">
-        <f t="shared" si="7"/>
-        <v>8400</v>
-      </c>
-      <c r="G49" s="35">
-        <f t="shared" si="7"/>
-        <v>400</v>
-      </c>
+      <c r="A49" s="72" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="70"/>
+      <c r="D49" s="72" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" s="70"/>
+      <c r="G49" s="70"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="35">
-        <v>10000</v>
-      </c>
-      <c r="C50" s="35">
-        <f>$B$50/5*(5-C$52)+2000/5*(5-C$52+1)</f>
-        <v>10000</v>
-      </c>
-      <c r="D50" s="35">
-        <f t="shared" ref="D50:F50" si="8">$B$50/5*(5-D$52)+2000/5*(5-D$52+1)</f>
-        <v>7600</v>
-      </c>
-      <c r="E50" s="35">
-        <f t="shared" si="8"/>
-        <v>5200</v>
-      </c>
-      <c r="F50" s="35">
-        <f t="shared" si="8"/>
-        <v>2800</v>
-      </c>
-      <c r="G50" s="35">
-        <f>$B$50/5*(5-G$52)+2000/5*(5-G$52+1)</f>
-        <v>400</v>
-      </c>
+      <c r="A50" s="73">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="70"/>
+      <c r="D50" s="73">
+        <v>5</v>
+      </c>
+      <c r="E50" s="74">
+        <f>'[2]CapEx and Funding'!F14*0</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="70"/>
+      <c r="G50" s="70"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" s="35">
-        <v>3000</v>
-      </c>
-      <c r="C51" s="35">
-        <f>$B$51/5*(5-C$52)+3000/5*(5-C$52+1)</f>
-        <v>5400</v>
-      </c>
-      <c r="D51" s="35">
-        <f t="shared" ref="D51:G51" si="9">$B$51/5*(5-D$52)+3000/5*(5-D$52+1)</f>
-        <v>4200</v>
-      </c>
-      <c r="E51" s="35">
-        <f t="shared" si="9"/>
-        <v>3000</v>
-      </c>
-      <c r="F51" s="35">
-        <f t="shared" si="9"/>
-        <v>1800</v>
-      </c>
-      <c r="G51" s="35">
-        <f t="shared" si="9"/>
-        <v>600</v>
-      </c>
+      <c r="A51" s="73">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="70"/>
+      <c r="D51" s="73">
+        <v>10</v>
+      </c>
+      <c r="E51" s="74">
+        <f>'[2]CapEx and Funding'!F14*5/D51*1000000</f>
+        <v>80420000</v>
+      </c>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C52" s="60">
-        <v>1</v>
-      </c>
-      <c r="D52" s="60">
-        <v>2</v>
-      </c>
-      <c r="E52" s="60">
-        <v>3</v>
-      </c>
-      <c r="F52" s="60">
-        <v>4</v>
-      </c>
-      <c r="G52" s="60">
-        <v>5</v>
-      </c>
+      <c r="A52" s="70"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="71"/>
+      <c r="F52" s="71"/>
+      <c r="G52" s="71"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="B53" s="35">
-        <f>SUM(B49:B51)</f>
-        <v>51000</v>
-      </c>
-      <c r="C53" s="35">
-        <f t="shared" ref="C53:G53" si="10">SUM(C49:C51)</f>
-        <v>47800</v>
-      </c>
-      <c r="D53" s="35">
-        <f t="shared" si="10"/>
-        <v>36200</v>
-      </c>
-      <c r="E53" s="35">
-        <f t="shared" si="10"/>
-        <v>24600</v>
-      </c>
-      <c r="F53" s="35">
-        <f t="shared" si="10"/>
-        <v>13000</v>
-      </c>
-      <c r="G53" s="35">
-        <f t="shared" si="10"/>
-        <v>1400</v>
-      </c>
+      <c r="A53" s="67"/>
+      <c r="B53" s="70"/>
+      <c r="C53" s="70"/>
+      <c r="D53" s="70"/>
+      <c r="E53" s="70"/>
+      <c r="F53" s="70"/>
+      <c r="G53" s="70"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="36" t="s">
@@ -5017,16 +4640,16 @@
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="61">
+      <c r="C5" s="60">
         <f>I19</f>
-        <v>1822466.8957163054</v>
+        <v>1665217.6936692854</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="61">
+      <c r="C6" s="60">
         <f>I24</f>
         <v>158170.20000000001</v>
       </c>
@@ -5061,9 +4684,9 @@
       <c r="A7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="62">
+      <c r="C7" s="61">
         <f>C5-C6</f>
-        <v>1664296.6957163054</v>
+        <v>1507047.4936692854</v>
       </c>
       <c r="K7" s="24" t="s">
         <v>34</v>
@@ -5098,18 +4721,18 @@
         <v>31</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="63">
+      <c r="C8" s="62">
         <f>C5/C6</f>
-        <v>11.522188729079847</v>
+        <v>10.528011557608735</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="63">
         <f>C7/S22</f>
-        <v>16.504330580288631</v>
+        <v>14.944937462011953</v>
       </c>
       <c r="D9" t="s">
         <v>56</v>
@@ -5433,62 +5056,62 @@
       </c>
       <c r="C18" s="27">
         <f>'Economic Data and Calculations'!B53*'Cost-Benefit Analysis'!M7</f>
-        <v>51000</v>
+        <v>0</v>
       </c>
       <c r="D18" s="27">
         <f>'Economic Data and Calculations'!C53*'Cost-Benefit Analysis'!N7</f>
-        <v>44454</v>
+        <v>0</v>
       </c>
       <c r="E18" s="27">
         <f>'Economic Data and Calculations'!D53*'Cost-Benefit Analysis'!O7</f>
-        <v>31309.379999999997</v>
+        <v>0</v>
       </c>
       <c r="F18" s="27">
         <f>'Economic Data and Calculations'!E53*'Cost-Benefit Analysis'!P7</f>
-        <v>19787.182199999996</v>
+        <v>0</v>
       </c>
       <c r="G18" s="27">
         <f>'Economic Data and Calculations'!F53*'Cost-Benefit Analysis'!Q7</f>
-        <v>9724.6761299999962</v>
+        <v>0</v>
       </c>
       <c r="H18" s="27">
         <f>'Economic Data and Calculations'!G53*'Cost-Benefit Analysis'!R7</f>
-        <v>973.96371701999965</v>
+        <v>0</v>
       </c>
       <c r="I18" s="27">
         <f t="shared" si="2"/>
-        <v>157249.20204701999</v>
+        <v>0</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>41</v>
       </c>
       <c r="M18" s="16">
         <f>'Economic Data and Calculations'!B53</f>
-        <v>51000</v>
+        <v>0</v>
       </c>
       <c r="N18" s="16">
         <f>'Economic Data and Calculations'!C53</f>
-        <v>47800</v>
+        <v>0</v>
       </c>
       <c r="O18" s="16">
         <f>'Economic Data and Calculations'!D53</f>
-        <v>36200</v>
+        <v>0</v>
       </c>
       <c r="P18" s="16">
         <f>'Economic Data and Calculations'!E53</f>
-        <v>24600</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="16">
         <f>'Economic Data and Calculations'!F53</f>
-        <v>13000</v>
+        <v>0</v>
       </c>
       <c r="R18" s="16">
         <f>'Economic Data and Calculations'!G53</f>
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="S18" s="16">
         <f t="shared" si="3"/>
-        <v>174000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
@@ -5497,62 +5120,62 @@
       </c>
       <c r="C19" s="23">
         <f>SUM(C14:C18)</f>
-        <v>77043.199999999997</v>
+        <v>26043.200000000001</v>
       </c>
       <c r="D19" s="23">
         <f t="shared" ref="D19:I19" si="4">SUM(D14:D18)</f>
-        <v>224914.17600000001</v>
+        <v>180460.17600000001</v>
       </c>
       <c r="E19" s="23">
         <f t="shared" si="4"/>
-        <v>357414.04367999994</v>
+        <v>326104.66367999994</v>
       </c>
       <c r="F19" s="23">
         <f t="shared" si="4"/>
-        <v>390630.50742239988</v>
+        <v>370843.3252223999</v>
       </c>
       <c r="G19" s="23">
         <f t="shared" si="4"/>
-        <v>392310.78989083192</v>
+        <v>382586.11376083194</v>
       </c>
       <c r="H19" s="23">
         <f t="shared" si="4"/>
-        <v>380154.17872307368</v>
+        <v>379180.21500605368</v>
       </c>
       <c r="I19" s="23">
         <f t="shared" si="4"/>
-        <v>1822466.8957163054</v>
+        <v>1665217.6936692854</v>
       </c>
       <c r="K19" s="23" t="s">
         <v>2</v>
       </c>
       <c r="M19" s="23">
         <f>SUM(M14:M18)</f>
-        <v>26094200</v>
+        <v>26043200</v>
       </c>
       <c r="N19" s="23">
         <f t="shared" ref="N19:Q19" si="5">SUM(N14:N18)</f>
-        <v>26259000</v>
+        <v>26211200</v>
       </c>
       <c r="O19" s="23">
         <f t="shared" si="5"/>
-        <v>26430400</v>
+        <v>26394200</v>
       </c>
       <c r="P19" s="23">
         <f t="shared" si="5"/>
-        <v>26502800</v>
+        <v>26478200</v>
       </c>
       <c r="Q19" s="23">
         <f t="shared" si="5"/>
-        <v>26541600</v>
+        <v>26528600</v>
       </c>
       <c r="R19" s="23">
         <f t="shared" ref="R19" si="6">SUM(R14:R18)</f>
-        <v>26563600</v>
+        <v>26562200</v>
       </c>
       <c r="S19" s="23">
         <f t="shared" ref="S19" si="7">SUM(S14:S18)</f>
-        <v>158391600</v>
+        <v>158217600</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Provide advice to the Minister
</commit_message>
<xml_diff>
--- a/Opal Lakes Dropbear Conservation Park.xlsx
+++ b/Opal Lakes Dropbear Conservation Park.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F11085-2B93-144A-B243-CCDC6A3F60F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C64172D-E95B-9C49-94E7-252520B47309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="DiscountRate">[1]Parameters!$C$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Economic Data and Calculations'!$A$1:$Q$116</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Minister Brief'!$A$1:$R$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Minister Brief'!$A$1:$R$47</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="139">
   <si>
     <t>Source</t>
   </si>
@@ -374,6 +374,90 @@
   </si>
   <si>
     <t>Discount rate</t>
+  </si>
+  <si>
+    <t>$ '000</t>
+  </si>
+  <si>
+    <t>Assumptions</t>
+  </si>
+  <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>Proponent can fund their portion of CapEx.</t>
+  </si>
+  <si>
+    <t>BCR</t>
+  </si>
+  <si>
+    <t>CapEx and Operations overlap, so 6 year analysis period.</t>
+  </si>
+  <si>
+    <t>NPV/I</t>
+  </si>
+  <si>
+    <t>Avoided costs only apply for 4 years as the Opal Lakes Volunteer Brigade only ceases functioning once construction is fully complete.</t>
+  </si>
+  <si>
+    <t>Yes, three.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPP17-03 states that a discount rate sensitivity rate should be included. </t>
+  </si>
+  <si>
+    <t>Consumer surplus sensitivity has been included as it has a strong impact on the CBA results, it is material at 95% confidence interval lower bound.</t>
+  </si>
+  <si>
+    <t>Central estimate = $10 per household</t>
+  </si>
+  <si>
+    <t>Sensitivity 1 = $7.5 per household</t>
+  </si>
+  <si>
+    <t>Sensitivity 2 = $12 per household</t>
+  </si>
+  <si>
+    <t>Asset life</t>
+  </si>
+  <si>
+    <t>5 years</t>
+  </si>
+  <si>
+    <t>10 years</t>
+  </si>
+  <si>
+    <t>If asset life can be extended then there is a strong positive impact on CBA results.</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t>Consumer surplus, source data from rigorous WTP survey results that avoids double counting with avoided costs below.</t>
+  </si>
+  <si>
+    <t>Producer surplus, induced visitation from interstate and international.</t>
+  </si>
+  <si>
+    <t>Labour surplus, induced visitation from interstate and international.</t>
+  </si>
+  <si>
+    <t>Avoided costs to NSW residents (Opal Lakes Volunteer Brigade), these are separate to below calculations of consumer, producer and labour surplus.</t>
+  </si>
+  <si>
+    <t>Proponent surplus (Residual asset value to Opal Lakes Shire Council)</t>
+  </si>
+  <si>
+    <t>CapEx to NSW Government and Council, both 100% NSW-owned.</t>
+  </si>
+  <si>
+    <t>Excluded</t>
+  </si>
+  <si>
+    <t>The proponent claims visitation by NSW residents. They have not provided a reliable source for estimated visitation, have made up the nightly spend and this has double counting with the WTP survey results for consumer surplus.</t>
   </si>
 </sst>
 </file>
@@ -582,7 +666,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -656,6 +740,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE6E6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,7 +969,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1037,6 +1133,31 @@
     <xf numFmtId="10" fontId="14" fillId="0" borderId="9" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="9" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="16" fillId="0" borderId="9" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="9" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Bad 2" xfId="1" xr:uid="{B03EBECC-4434-4525-8FB0-19D98432DF3E}"/>
@@ -1058,21 +1179,21 @@
   <dxfs count="8">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1108,21 +1229,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2279,7 +2400,30 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="3">
+        <row r="2">
+          <cell r="M2">
+            <v>10</v>
+          </cell>
+          <cell r="N2">
+            <v>7.5</v>
+          </cell>
+          <cell r="O2">
+            <v>12</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="M3">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+          <cell r="N3">
+            <v>0.03</v>
+          </cell>
+          <cell r="O3">
+            <v>0.1</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
@@ -4679,8 +4823,8 @@
   </sheetPr>
   <dimension ref="A1:S167"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8532,26 +8676,26 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>IF($C$8&lt;1, TRUE, FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>IF(C8&gt;1, TRUE, FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
-      <formula>IF($C$8&lt;1, TRUE, FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>IF(C9&gt;0, TRUE, FALSE)</formula>
-    </cfRule>
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>IF(C9&lt;0, TRUE, FALSE)</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>IF(C9&gt;0, TRUE, FALSE)</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>IF(C7&lt;0, TRUE, FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>IF(C7&gt;0, TRUE, FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8588,9 +8732,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U46"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8603,26 +8749,22 @@
     <col min="11" max="11" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -8636,11 +8778,13 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C5" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -8654,11 +8798,16 @@
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="91">
+        <v>5155.2773394444084</v>
+      </c>
+      <c r="E6" t="s">
+        <v>114</v>
+      </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -8672,11 +8821,16 @@
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="60">
+        <v>1.0325572762231112</v>
+      </c>
+      <c r="E7" t="s">
+        <v>116</v>
+      </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -8690,11 +8844,16 @@
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="60">
+        <v>5.1928920148008872E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
@@ -8708,238 +8867,260 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
+      <c r="H10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="92">
+        <f>'[2]Cost-Benefit Analysis'!N3</f>
+        <v>0.03</v>
+      </c>
+      <c r="E11" s="92">
+        <f>'[2]Cost-Benefit Analysis'!M3</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F11" s="92">
+        <f>'[2]Cost-Benefit Analysis'!O3</f>
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="93">
+        <v>22641.673201955244</v>
+      </c>
+      <c r="E12" s="93">
+        <v>5155.2773394444084</v>
+      </c>
+      <c r="F12" s="93">
+        <v>-5949.3681926843419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="94">
+        <v>1.1417504354946415</v>
+      </c>
+      <c r="E13" s="94">
+        <v>1.0325572762231112</v>
+      </c>
+      <c r="F13" s="94">
+        <v>0.96219568475563066</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="94">
+        <v>0.22609222575325397</v>
+      </c>
+      <c r="E14" s="94">
+        <v>5.1928920148008872E-2</v>
+      </c>
+      <c r="F14" s="94">
+        <v>-6.0297957793577599E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C16" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="95">
+        <f>'[2]Cost-Benefit Analysis'!N2</f>
+        <v>7.5</v>
+      </c>
+      <c r="E16" s="95">
+        <f>'[2]Cost-Benefit Analysis'!M2</f>
+        <v>10</v>
+      </c>
+      <c r="F16" s="95">
+        <f>'[2]Cost-Benefit Analysis'!O2</f>
+        <v>12</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
+      <c r="C17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="93">
+        <v>-1355.522660555609</v>
+      </c>
+      <c r="E17" s="93">
+        <v>5155.2773394444084</v>
+      </c>
+      <c r="F17" s="93">
+        <v>10363.917339444393</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
+      <c r="C18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="96">
+        <v>0.99143942744869828</v>
+      </c>
+      <c r="E18" s="94">
+        <v>1.0325572762231112</v>
+      </c>
+      <c r="F18" s="96">
+        <v>1.0654515552426416</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
+      <c r="C19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="96">
+        <v>-1.3654130197851758E-2</v>
+      </c>
+      <c r="E19" s="94">
+        <v>5.1928920148008872E-2</v>
+      </c>
+      <c r="F19" s="96">
+        <v>0.10439536042469709</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
+      <c r="C21" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="97" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="97" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="40"/>
+      <c r="H21" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="C22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="93">
+        <v>5155.2773394444084</v>
+      </c>
+      <c r="E22" s="93">
+        <v>62493.625893521035</v>
+      </c>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
@@ -8949,15 +9130,15 @@
       <c r="Q22" s="13"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
+      <c r="C23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="94">
+        <v>1.0325572762231112</v>
+      </c>
+      <c r="E23" s="96">
+        <v>1.3946678532368575</v>
+      </c>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
@@ -8967,15 +9148,15 @@
       <c r="Q23" s="13"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
+      <c r="C24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="94">
+        <v>5.1928920148008872E-2</v>
+      </c>
+      <c r="E24" s="96">
+        <v>0.62949600867330568</v>
+      </c>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
@@ -8985,32 +9166,29 @@
       <c r="Q24" s="13"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-    </row>
-    <row r="27" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -9032,245 +9210,145 @@
       <c r="U27" s="13"/>
     </row>
     <row r="28" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
+      <c r="B28" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="99" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="98"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="100"/>
+      <c r="M28" s="100"/>
+      <c r="N28" s="100"/>
+      <c r="O28" s="100"/>
+      <c r="P28" s="100"/>
+      <c r="Q28" s="100"/>
+      <c r="R28" s="100"/>
+      <c r="S28" s="100"/>
+      <c r="T28" s="100"/>
       <c r="U28" s="13"/>
     </row>
     <row r="29" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13"/>
+      <c r="C29" s="101">
+        <v>26043.200000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>131</v>
+      </c>
+      <c r="J29" s="93"/>
       <c r="U29" s="13"/>
     </row>
     <row r="30" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
+      <c r="C30" s="101">
+        <v>40487.70024094484</v>
+      </c>
+      <c r="D30" t="s">
+        <v>132</v>
+      </c>
+      <c r="J30" s="93"/>
       <c r="U30" s="13"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
+    <row r="31" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="101">
+        <v>49484.966961154802</v>
+      </c>
+      <c r="D31" t="s">
+        <v>133</v>
+      </c>
+      <c r="J31" s="93"/>
       <c r="U31" s="13"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13"/>
+      <c r="C32" s="101">
+        <v>47484.269950428854</v>
+      </c>
+      <c r="D32" t="s">
+        <v>134</v>
+      </c>
+      <c r="J32" s="93"/>
       <c r="U32" s="13"/>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13"/>
+      <c r="C33" s="101">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" s="93"/>
       <c r="U33" s="13"/>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
-      <c r="T34" s="13"/>
       <c r="U34" s="13"/>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13"/>
+      <c r="B35" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="103"/>
+      <c r="D35" s="103"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="103"/>
+      <c r="H35" s="103"/>
+      <c r="I35" s="103"/>
+      <c r="J35" s="103"/>
+      <c r="K35" s="103"/>
+      <c r="L35" s="103"/>
+      <c r="M35" s="103"/>
+      <c r="N35" s="103"/>
+      <c r="O35" s="103"/>
+      <c r="P35" s="103"/>
+      <c r="Q35" s="103"/>
+      <c r="R35" s="103"/>
+      <c r="S35" s="103"/>
+      <c r="T35" s="103"/>
       <c r="U35" s="13"/>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13"/>
-      <c r="T36" s="13"/>
+      <c r="C36" s="93">
+        <v>158344.8598130841</v>
+      </c>
+      <c r="D36" t="s">
+        <v>136</v>
+      </c>
+      <c r="J36" s="93"/>
       <c r="U36" s="13"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="13"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="13"/>
-      <c r="T37" s="13"/>
       <c r="U37" s="13"/>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-      <c r="Q38" s="13"/>
-      <c r="R38" s="13"/>
-      <c r="S38" s="13"/>
-      <c r="T38" s="13"/>
+      <c r="B38" s="69" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="104" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38" s="104"/>
+      <c r="E38" s="104"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="104"/>
+      <c r="H38" s="104"/>
+      <c r="I38" s="104"/>
+      <c r="J38" s="104"/>
+      <c r="K38" s="104"/>
+      <c r="L38" s="104"/>
+      <c r="M38" s="104"/>
+      <c r="N38" s="104"/>
+      <c r="O38" s="104"/>
+      <c r="P38" s="104"/>
+      <c r="Q38" s="104"/>
+      <c r="R38" s="104"/>
+      <c r="S38" s="104"/>
+      <c r="T38" s="104"/>
       <c r="U38" s="13"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.2">
@@ -9448,6 +9526,28 @@
       <c r="S46" s="13"/>
       <c r="T46" s="13"/>
       <c r="U46" s="13"/>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>